<commit_message>
added column to Price excel sheet to include the cost attribute
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.price.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.price.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Pack</t>
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
   <si>
     <t>Date Added</t>
@@ -384,16 +387,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="30.7109375" customWidth="1"/>
+    <col min="1" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,74 +409,92 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>25</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3">
         <v>44228</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="E2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3">
         <v>44228</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>12</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
+        <v>7.77</v>
+      </c>
+      <c r="D4" s="3">
         <v>44228</v>
       </c>
-      <c r="D4" s="2" t="b">
+      <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>65</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
+        <v>46.86</v>
+      </c>
+      <c r="D5" s="3">
         <v>44228</v>
       </c>
-      <c r="D5" s="2" t="b">
+      <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
         <v>44228</v>
       </c>
-      <c r="D6" s="2" t="b">
+      <c r="E6" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added larger data set
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.price.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.price.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Pack</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,7 +427,7 @@
         <v>44231</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -461,6 +461,40 @@
         <v>44231</v>
       </c>
       <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44231</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44231</v>
+      </c>
+      <c r="E6" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>